<commit_message>
draft version for release
</commit_message>
<xml_diff>
--- a/data/Target reflectivities.xlsx
+++ b/data/Target reflectivities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7741507C-8C4C-45FA-A1C2-719536819C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7CD07F-FBB8-4CD1-88F4-AD70B0B77A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2186" yWindow="1389" windowWidth="23914" windowHeight="16285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,10 +476,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R109"/>
+  <dimension ref="A1:O109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -499,10 +499,9 @@
     <col min="13" max="13" width="12.69921875" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.19921875" style="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -548,11 +547,8 @@
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>0.3</v>
       </c>
@@ -599,7 +595,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>0.31</v>
       </c>
@@ -646,7 +642,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>0.32</v>
       </c>
@@ -693,7 +689,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>0.33</v>
       </c>
@@ -740,7 +736,7 @@
         <v>6.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>0.34</v>
       </c>
@@ -787,7 +783,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>0.35</v>
       </c>
@@ -834,7 +830,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>0.36</v>
       </c>
@@ -881,7 +877,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>0.37</v>
       </c>
@@ -928,7 +924,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>0.38</v>
       </c>
@@ -975,7 +971,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>0.39</v>
       </c>
@@ -1022,7 +1018,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>0.4</v>
       </c>
@@ -1069,7 +1065,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>0.41</v>
       </c>
@@ -1116,7 +1112,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>0.42</v>
       </c>
@@ -1163,7 +1159,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>0.43</v>
       </c>
@@ -1210,7 +1206,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>0.44</v>
       </c>
@@ -5017,7 +5013,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>1.25</v>
       </c>
@@ -5064,7 +5060,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>1.26</v>
       </c>
@@ -5111,7 +5107,7 @@
         <v>0.13200000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>1.27</v>
       </c>
@@ -5158,7 +5154,7 @@
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>1.28</v>
       </c>
@@ -5205,7 +5201,7 @@
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>1.29</v>
       </c>
@@ -5252,7 +5248,7 @@
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>1.3</v>
       </c>
@@ -5299,7 +5295,7 @@
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:18" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -5315,11 +5311,8 @@
       <c r="M105" s="8"/>
       <c r="N105" s="8"/>
       <c r="O105" s="8"/>
-      <c r="P105" s="7"/>
-      <c r="Q105" s="7"/>
-      <c r="R105" s="7"/>
-    </row>
-    <row r="106" spans="1:18" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:15" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -5335,11 +5328,8 @@
       <c r="M106" s="8"/>
       <c r="N106" s="8"/>
       <c r="O106" s="8"/>
-      <c r="P106" s="7"/>
-      <c r="Q106" s="7"/>
-      <c r="R106" s="7"/>
-    </row>
-    <row r="107" spans="1:18" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:15" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
       <c r="A107" s="9"/>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -5355,11 +5345,8 @@
       <c r="M107" s="8"/>
       <c r="N107" s="8"/>
       <c r="O107" s="8"/>
-      <c r="P107" s="7"/>
-      <c r="Q107" s="7"/>
-      <c r="R107" s="7"/>
-    </row>
-    <row r="108" spans="1:18" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:15" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -5375,11 +5362,8 @@
       <c r="M108" s="8"/>
       <c r="N108" s="8"/>
       <c r="O108" s="8"/>
-      <c r="P108" s="7"/>
-      <c r="Q108" s="7"/>
-      <c r="R108" s="7"/>
-    </row>
-    <row r="109" spans="1:18" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:15" s="1" customFormat="1" ht="10.3" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
@@ -5395,9 +5379,6 @@
       <c r="M109" s="8"/>
       <c r="N109" s="8"/>
       <c r="O109" s="8"/>
-      <c r="P109" s="7"/>
-      <c r="Q109" s="7"/>
-      <c r="R109" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>